<commit_message>
ctuko polyseq; read in data
</commit_message>
<xml_diff>
--- a/input/other/IDT_barcodes.xlsx
+++ b/input/other/IDT_barcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kate/Documents/Working_hub/Chevrier_Lab/Projects/U01/Code/Git_Hub/polysome-seq/input/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47134220-C270-A748-B1D0-0E5CBB0AC526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229E9D07-9C9A-B547-9886-C709DC88F651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="12800" xr2:uid="{9550E013-F852-FF4C-8958-AE0585AD8478}"/>
   </bookViews>
@@ -1554,10 +1554,13 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:M38"/>
+      <selection activeCell="B23" sqref="B23:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>